<commit_message>
adding maintainance for bike/elliptical
</commit_message>
<xml_diff>
--- a/Python/PIP_GEN_id-0/Parts - Consoles.csv.xlsx
+++ b/Python/PIP_GEN_id-0/Parts - Consoles.csv.xlsx
@@ -1033,7 +1033,7 @@
         <v>75</v>
       </c>
       <c r="BA2" s="2" t="n">
-        <v>43123.71864396991</v>
+        <v>43124.50381199074</v>
       </c>
     </row>
   </sheetData>
@@ -1164,7 +1164,7 @@
         <v>98</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>43123.71859715278</v>
+        <v>43124.50379405093</v>
       </c>
       <c r="C8" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Bike and Elliptical is needed
</commit_message>
<xml_diff>
--- a/Python/PIP_GEN_id-0/Parts - Consoles.csv.xlsx
+++ b/Python/PIP_GEN_id-0/Parts - Consoles.csv.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
   <si>
     <t>RecordID</t>
   </si>
@@ -177,21 +177,31 @@
     <t>Created</t>
   </si>
   <si>
-    <t>387469</t>
-  </si>
-  <si>
-    <t>ETFM39817</t>
+    <t>385843</t>
+  </si>
+  <si>
+    <t>ETNT22116</t>
   </si>
   <si>
     <t>TREADMILL_DEVICE</t>
   </si>
   <si>
-    <t>FENDER_DISPLAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">将电源线连接到EQF1259，将EQW1053的一端连接到EQF1259（CLUB）。注意：请确保您选择与控制台类型相匹配的正确端口。将地线（绿色）连接到E-GND EQF 1259.设置夹具配置：使用PC，在控制台名称（例如：... RNDFtp \ EBNT02117 \ Procedure）下载入RNDftp中的.xml配置文件到microSD卡，将microSD卡正面朝上插入microSD打开灯具背面的RESET按钮，使用UP和DOWN按钮找到合适的配置文件，按ENTER键选择配置文件（屏幕1），等待5秒钟，屏幕稳定后设置灯具脉冲：按下EQF1259 2x上的显示按下此灯具上的开始使用上下按钮设置一个随机脉冲，按下灯具上的开始，按下显示一次。
+    <t>NO_DISPLAY</t>
+  </si>
+  <si>
+    <t>“EQF1259控制台夹具
+PC w /访问RNDftp
+MicroSD卡“
+EQW1001; 8针线束
+EQF1259 Console Fixture
+PC w/ Access to RNDftp
+MicroSD Card
+EQW1001; 8-pin harness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“将电源线连接到EQF1259，将EQW1001的一端连接到EQF1259（TRED1）。注意：请确保您选择与控制台类型相匹配的正确端口。将地线（绿色）连接到E-GND EQF 1259.设置夹具配置：使用PC，在控制台名称（例如：... RNDFtp \ EBNT02117 \ Procedure）下载入RNDftp中的.xml配置文件到microSD卡，将microSD卡正面朝上插入microSD打开灯具背面的RESET按钮，使用UP和DOWN按钮找到合适的配置文件，按ENTER键选择配置文件（屏幕1），等待5秒钟，屏幕稳定后设置灯具脉冲：按下EQF1259 2x上的显示按下此灯具上的开始使用上下按钮设置一个随机脉冲，按下灯具上的开始，按下显示一次。
 Connect the power cord to the EQF1259. 
-Connect one end of the EQW1053 to EQF1259 (CLUB). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
+Connect one end of the EQW1001 to EQF1259 (TRED1). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
 Connect the ground wire (Green) to E-GND on EQF 1259. 
 Set Fixture Configurations:
 Using PC, load .xml configuration file, which is found in the RNDftp under the console name (Example: …RNDFtp\EBNT02117\Procedure) to the microSD card.
@@ -217,19 +227,51 @@
 Verify that the General Warning is printed on the console or pulse bar.</t>
   </si>
   <si>
-    <t xml:space="preserve">“确保设备包装在防静电袋中，目视检查控制台是否有化妆品缺陷，物理损坏和不清晰的打印。
+    <t>检查控制台是否与图片一致如果数位板倾斜，验证倾斜是否平稳移动，保持位置，并旋转全程。
 Ensure the unit is packaged in an antistatic bag. 
 Visually inspect the console for cosmetic defects, physical damage, and illegible printing.  
 Verify console matches picture
-</t>
-  </si>
-  <si>
-    <t>将14针MTA连接到控制台。在EQF1259上，打开控制台电源开关。
-Connect the 14-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
+If tablet has tilt, verify tilt  is smooth moving, holds position, and rotates through full range.</t>
+  </si>
+  <si>
+    <t>将8针MTA连接到控制台。在EQF1259上，打开控制台电源开关。
+Connect the 8-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
   </si>
   <si>
     <t>将死者的钥匙插入控制台。
 Insert Dead Man Key into console.</t>
+  </si>
+  <si>
+    <t>触摸屏幕右下方的用户个人资料图标
+触摸设置
+触摸“设备信息”，然后点击“应用程序信息”。 这将显示应用程序版本和Brainboard版本。
+验证和记录。
+按下数位板上的后退箭头返回到主屏幕
+Touch user profile icon at the lower right  of the screen
+Touch settings
+Touch “Equipment Info” and then “App Info”. This will display App version and Brainboard version.
+Verify and Record.
+Press the back arrow on the tablet to return to main screen</t>
+  </si>
+  <si>
+    <t>触摸屏幕右下方的用户配置文件图标
+触摸设置
+触摸维护
+选择校准倾斜
+在EQF1259上按Calibrate
+按开始在平板电脑上开始倾斜校准。 确认显示屏上的倾斜值短暂增加，暂停，然后减小到零
+校准完成后，按下数位板上的后退箭头返回主屏幕“
+Touch the user profile icon on lower right of the screen
+Touch Settings
+Touch Maintainance
+Select Calibrate Incline
+Press Calibrate on EQF1259
+Press Begin on tablet to start incline calibration.  Verify the incline value on the display increases briefly, pauses, then decrease to zero
+When calibration is complete, press the back arrow on the tablet to return to main screen</t>
+  </si>
+  <si>
+    <t>验证平板电脑显示屏是否亮起且没有缺陷
+Verify tablet display is lit and without flaws</t>
   </si>
   <si>
     <t>“在控制台上，按随机快速按钮。
@@ -246,6 +288,20 @@
   <si>
     <t>将EQF1259的USB电缆插入控制台，并确认EQF1259上显示“USB”。
 Plug USB cable from EQF1259 into console and verify "USB" is displayed on the EQF1259.</t>
+  </si>
+  <si>
+    <t>保持脉冲条并确认显示脉冲读数
+Hold the pulse bars and verify a pulse reading is displayed</t>
+  </si>
+  <si>
+    <t>按显示按钮，进入BLE脉冲屏幕。
+按开始按钮。
+在控制台上运行手动锻炼。
+验证在控制台上读取脉冲BLE脉冲。“
+Press Display button to goto BLE Pulse screen.
+Press Start button.
+Run manual workout on the console.
+Verify pulse BLE pulse is read on console.</t>
   </si>
   <si>
     <t>“将3针风扇连接到控制台。
@@ -258,6 +314,20 @@
 Press the Small Fan button to turn fan to low, then press again to turn fan off.</t>
   </si>
   <si>
+    <t>“将EQW1007连接到iOS音频源，并将EQW1007的另一端连接到控制台。
+播放音频并验证它是否从控制台扬声器播放。
+调整音量到最低和最高水平，并验证一个变化。“
+Connect the EQW1007 to the iOS audio source and connect the other end of the EQW1007 to the console.
+Play audio and verify that it plays out of the console speakers.
+Adjust the volume to minimum and maximum level and verify a change.</t>
+  </si>
+  <si>
+    <t>“将HDMI电缆连接到电视机。
+将HDMI电缆连接到控制台，控制台屏幕和声音将在电视上镜像。“
+Connect the HDMI cable to the TV.
+Connect the HDMI cable to the console and the console screen and sound will be mirrored on the TV.</t>
+  </si>
+  <si>
     <t>“在EQF1259上，关闭控制台电源。
 断开控制台上的所有电线和电缆。“
 On the EQF1259, turn off the Console power.
@@ -276,16 +346,19 @@
     <t>From chaos, springs new beginnings!</t>
   </si>
   <si>
+    <t>LOKI</t>
+  </si>
+  <si>
+    <t>REV 1</t>
+  </si>
+  <si>
+    <t>20171205</t>
+  </si>
+  <si>
+    <t>Created arrays for variables</t>
+  </si>
+  <si>
     <t>id-0</t>
-  </si>
-  <si>
-    <t>REV 1</t>
-  </si>
-  <si>
-    <t>20171205</t>
-  </si>
-  <si>
-    <t>Created arrays for variables</t>
   </si>
   <si>
     <t>REV 2</t>
@@ -915,44 +988,68 @@
       <c r="G2" t="s">
         <v>56</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="AY2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="BA2" s="2" t="n">
-        <v>43151.7145949537</v>
+        <v>43153.48585454861</v>
       </c>
     </row>
   </sheetData>
@@ -982,114 +1079,114 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>43151.71090541666</v>
+        <v>43153.48395670139</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>